<commit_message>
add financial report download
</commit_message>
<xml_diff>
--- a/src/main/resources/Financial_Report_2021.xlsx
+++ b/src/main/resources/Financial_Report_2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Works\projects\church-app\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38A0303C-8C9A-4E74-9D1E-0B661779A495}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9565A56-628C-4EB3-A1CC-2B299F5CE44E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15990" xr2:uid="{7F8DEBD6-32E0-4BF8-87C4-D1C13E633F04}"/>
+    <workbookView xWindow="980" yWindow="0" windowWidth="13740" windowHeight="10800" xr2:uid="{7F8DEBD6-32E0-4BF8-87C4-D1C13E633F04}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="252">
   <si>
     <t>Alpha Korean United Church</t>
   </si>
@@ -1341,6 +1341,9 @@
     </xf>
     <xf numFmtId="4" fontId="6" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="6" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1443,33 +1446,30 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1791,7 +1791,7 @@
   <dimension ref="A1:K35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="A4" sqref="A4:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1811,88 +1811,88 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18.5">
-      <c r="A1" s="111" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="111"/>
-      <c r="C1" s="112"/>
-      <c r="D1" s="112"/>
-      <c r="E1" s="112"/>
-      <c r="F1" s="113"/>
-      <c r="G1" s="113"/>
-      <c r="H1" s="113"/>
-      <c r="I1" s="113"/>
-      <c r="J1" s="113"/>
-      <c r="K1" s="113"/>
+      <c r="A1" s="112" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="112"/>
+      <c r="C1" s="113"/>
+      <c r="D1" s="113"/>
+      <c r="E1" s="113"/>
+      <c r="F1" s="114"/>
+      <c r="G1" s="114"/>
+      <c r="H1" s="114"/>
+      <c r="I1" s="114"/>
+      <c r="J1" s="114"/>
+      <c r="K1" s="114"/>
     </row>
     <row r="2" spans="1:11" ht="18.5">
-      <c r="A2" s="111" t="s">
-        <v>235</v>
-      </c>
-      <c r="B2" s="112"/>
-      <c r="C2" s="112"/>
-      <c r="D2" s="112"/>
-      <c r="E2" s="112"/>
-      <c r="F2" s="113"/>
-      <c r="G2" s="113"/>
-      <c r="H2" s="113"/>
-      <c r="I2" s="113"/>
-      <c r="J2" s="113"/>
-      <c r="K2" s="113"/>
+      <c r="A2" s="112" t="s">
+        <v>239</v>
+      </c>
+      <c r="B2" s="113"/>
+      <c r="C2" s="113"/>
+      <c r="D2" s="113"/>
+      <c r="E2" s="113"/>
+      <c r="F2" s="114"/>
+      <c r="G2" s="114"/>
+      <c r="H2" s="114"/>
+      <c r="I2" s="114"/>
+      <c r="J2" s="114"/>
+      <c r="K2" s="114"/>
     </row>
     <row r="3" spans="1:11" ht="18.5">
-      <c r="A3" s="114" t="s">
-        <v>239</v>
-      </c>
-      <c r="B3" s="114"/>
-      <c r="C3" s="112"/>
-      <c r="D3" s="112"/>
-      <c r="E3" s="112"/>
-      <c r="F3" s="113"/>
-      <c r="G3" s="113"/>
-      <c r="H3" s="113"/>
-      <c r="I3" s="113"/>
-      <c r="J3" s="113"/>
-      <c r="K3" s="113"/>
+      <c r="A3" s="115">
+        <v>2021</v>
+      </c>
+      <c r="B3" s="115"/>
+      <c r="C3" s="113"/>
+      <c r="D3" s="113"/>
+      <c r="E3" s="113"/>
+      <c r="F3" s="114"/>
+      <c r="G3" s="114"/>
+      <c r="H3" s="114"/>
+      <c r="I3" s="114"/>
+      <c r="J3" s="114"/>
+      <c r="K3" s="114"/>
     </row>
     <row r="4" spans="1:11">
-      <c r="A4" s="119" t="s">
+      <c r="A4" s="120" t="s">
         <v>237</v>
       </c>
-      <c r="B4" s="120"/>
-      <c r="C4" s="121"/>
-      <c r="D4" s="121"/>
-      <c r="E4" s="122"/>
-      <c r="G4" s="106" t="s">
+      <c r="B4" s="121"/>
+      <c r="C4" s="122"/>
+      <c r="D4" s="122"/>
+      <c r="E4" s="123"/>
+      <c r="G4" s="107" t="s">
         <v>240</v>
       </c>
-      <c r="H4" s="107"/>
-      <c r="I4" s="107"/>
-      <c r="J4" s="107"/>
-      <c r="K4" s="108"/>
+      <c r="H4" s="108"/>
+      <c r="I4" s="108"/>
+      <c r="J4" s="108"/>
+      <c r="K4" s="109"/>
     </row>
     <row r="5" spans="1:11">
-      <c r="A5" s="123" t="s">
+      <c r="A5" s="124" t="s">
         <v>208</v>
       </c>
-      <c r="B5" s="124"/>
+      <c r="B5" s="125"/>
       <c r="C5" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="152" t="s">
+      <c r="D5" s="105" t="s">
         <v>5</v>
       </c>
       <c r="E5" s="81" t="s">
         <v>198</v>
       </c>
-      <c r="G5" s="109" t="s">
+      <c r="G5" s="110" t="s">
         <v>241</v>
       </c>
-      <c r="H5" s="110"/>
+      <c r="H5" s="111"/>
       <c r="I5" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="J5" s="152" t="s">
+      <c r="J5" s="105" t="s">
         <v>5</v>
       </c>
       <c r="K5" s="81" t="s">
@@ -2290,11 +2290,11 @@
         <f>Offering!$G$17</f>
         <v>0</v>
       </c>
-      <c r="G17" s="128"/>
-      <c r="H17" s="129"/>
-      <c r="I17" s="129"/>
-      <c r="J17" s="129"/>
-      <c r="K17" s="130"/>
+      <c r="G17" s="129"/>
+      <c r="H17" s="130"/>
+      <c r="I17" s="130"/>
+      <c r="J17" s="130"/>
+      <c r="K17" s="131"/>
     </row>
     <row r="18" spans="1:11">
       <c r="A18" s="82"/>
@@ -2388,10 +2388,10 @@
       <c r="K21" s="95"/>
     </row>
     <row r="22" spans="1:11">
-      <c r="A22" s="115" t="s">
+      <c r="A22" s="116" t="s">
         <v>225</v>
       </c>
-      <c r="B22" s="116"/>
+      <c r="B22" s="117"/>
       <c r="C22" s="19">
         <f t="shared" ref="C22:E22" si="2">SUBTOTAL(9,C6:C21)</f>
         <v>148000</v>
@@ -2422,11 +2422,11 @@
       </c>
     </row>
     <row r="23" spans="1:11">
-      <c r="A23" s="125"/>
-      <c r="B23" s="126"/>
-      <c r="C23" s="126"/>
-      <c r="D23" s="126"/>
-      <c r="E23" s="127"/>
+      <c r="A23" s="126"/>
+      <c r="B23" s="127"/>
+      <c r="C23" s="127"/>
+      <c r="D23" s="127"/>
+      <c r="E23" s="128"/>
       <c r="G23" s="99"/>
       <c r="H23" s="22" t="s">
         <v>245</v>
@@ -2572,10 +2572,10 @@
       </c>
     </row>
     <row r="28" spans="1:11">
-      <c r="A28" s="115" t="s">
+      <c r="A28" s="116" t="s">
         <v>228</v>
       </c>
-      <c r="B28" s="116"/>
+      <c r="B28" s="117"/>
       <c r="C28" s="19">
         <f>SUBTOTAL(9,C24:C27)</f>
         <v>15000</v>
@@ -2606,16 +2606,16 @@
       </c>
     </row>
     <row r="29" spans="1:11">
-      <c r="A29" s="125"/>
-      <c r="B29" s="126"/>
-      <c r="C29" s="126"/>
-      <c r="D29" s="126"/>
-      <c r="E29" s="127"/>
-      <c r="G29" s="131"/>
-      <c r="H29" s="129"/>
-      <c r="I29" s="129"/>
-      <c r="J29" s="129"/>
-      <c r="K29" s="130"/>
+      <c r="A29" s="126"/>
+      <c r="B29" s="127"/>
+      <c r="C29" s="127"/>
+      <c r="D29" s="127"/>
+      <c r="E29" s="128"/>
+      <c r="G29" s="132"/>
+      <c r="H29" s="130"/>
+      <c r="I29" s="130"/>
+      <c r="J29" s="130"/>
+      <c r="K29" s="131"/>
     </row>
     <row r="30" spans="1:11">
       <c r="A30" s="88" t="s">
@@ -2678,10 +2678,10 @@
       <c r="K32" s="98"/>
     </row>
     <row r="33" spans="1:11">
-      <c r="A33" s="117" t="s">
+      <c r="A33" s="118" t="s">
         <v>232</v>
       </c>
-      <c r="B33" s="118"/>
+      <c r="B33" s="119"/>
       <c r="C33" s="101">
         <f>SUBTOTAL(9,C6:C32)</f>
         <v>220490</v>
@@ -2694,10 +2694,10 @@
         <f>SUBTOTAL(9,E6:E32)</f>
         <v>0</v>
       </c>
-      <c r="G33" s="132" t="s">
+      <c r="G33" s="133" t="s">
         <v>248</v>
       </c>
-      <c r="H33" s="133"/>
+      <c r="H33" s="134"/>
       <c r="I33" s="103">
         <f>SUBTOTAL(9,I6:I28)</f>
         <v>220490</v>
@@ -2712,19 +2712,19 @@
       </c>
     </row>
     <row r="35" spans="1:11">
-      <c r="A35" s="105" t="s">
+      <c r="A35" s="106" t="s">
         <v>250</v>
       </c>
-      <c r="B35" s="105"/>
-      <c r="C35" s="105"/>
-      <c r="D35" s="105"/>
-      <c r="E35" s="105"/>
-      <c r="F35" s="105"/>
-      <c r="G35" s="105"/>
-      <c r="H35" s="105"/>
-      <c r="I35" s="105"/>
-      <c r="J35" s="105"/>
-      <c r="K35" s="105"/>
+      <c r="B35" s="106"/>
+      <c r="C35" s="106"/>
+      <c r="D35" s="106"/>
+      <c r="E35" s="106"/>
+      <c r="F35" s="106"/>
+      <c r="G35" s="106"/>
+      <c r="H35" s="106"/>
+      <c r="I35" s="106"/>
+      <c r="J35" s="106"/>
+      <c r="K35" s="106"/>
     </row>
   </sheetData>
   <mergeCells count="16">
@@ -2768,15 +2768,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="15.5">
-      <c r="A1" s="136" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="136"/>
-      <c r="C1" s="137"/>
-      <c r="D1" s="137"/>
-      <c r="E1" s="137"/>
-      <c r="F1" s="138"/>
-      <c r="G1" s="138"/>
+      <c r="A1" s="137" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="137"/>
+      <c r="C1" s="138"/>
+      <c r="D1" s="138"/>
+      <c r="E1" s="138"/>
+      <c r="F1" s="139"/>
+      <c r="G1" s="139"/>
       <c r="H1" s="8"/>
       <c r="I1" s="8"/>
       <c r="J1" s="8"/>
@@ -2791,15 +2791,15 @@
       <c r="S1" s="8"/>
     </row>
     <row r="2" spans="1:19" ht="15.5">
-      <c r="A2" s="136" t="s">
+      <c r="A2" s="137" t="s">
         <v>235</v>
       </c>
-      <c r="B2" s="138"/>
-      <c r="C2" s="138"/>
-      <c r="D2" s="138"/>
-      <c r="E2" s="138"/>
-      <c r="F2" s="138"/>
-      <c r="G2" s="138"/>
+      <c r="B2" s="139"/>
+      <c r="C2" s="139"/>
+      <c r="D2" s="139"/>
+      <c r="E2" s="139"/>
+      <c r="F2" s="139"/>
+      <c r="G2" s="139"/>
       <c r="H2" s="8"/>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
@@ -2814,15 +2814,15 @@
       <c r="S2" s="8"/>
     </row>
     <row r="3" spans="1:19" ht="15.5">
-      <c r="A3" s="139" t="s">
+      <c r="A3" s="140" t="s">
         <v>236</v>
       </c>
-      <c r="B3" s="139"/>
-      <c r="C3" s="137"/>
-      <c r="D3" s="137"/>
-      <c r="E3" s="137"/>
-      <c r="F3" s="138"/>
-      <c r="G3" s="138"/>
+      <c r="B3" s="140"/>
+      <c r="C3" s="138"/>
+      <c r="D3" s="138"/>
+      <c r="E3" s="138"/>
+      <c r="F3" s="139"/>
+      <c r="G3" s="139"/>
       <c r="H3" s="8"/>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -2837,10 +2837,10 @@
       <c r="S3" s="8"/>
     </row>
     <row r="4" spans="1:19">
-      <c r="A4" s="140" t="s">
+      <c r="A4" s="141" t="s">
         <v>237</v>
       </c>
-      <c r="B4" s="140"/>
+      <c r="B4" s="141"/>
       <c r="C4" s="30"/>
       <c r="D4" s="30"/>
       <c r="E4" s="31"/>
@@ -2860,10 +2860,10 @@
       <c r="S4" s="8"/>
     </row>
     <row r="5" spans="1:19">
-      <c r="A5" s="141" t="s">
+      <c r="A5" s="142" t="s">
         <v>208</v>
       </c>
-      <c r="B5" s="141"/>
+      <c r="B5" s="142"/>
       <c r="C5" s="34" t="s">
         <v>209</v>
       </c>
@@ -3475,10 +3475,10 @@
       <c r="S21" s="8"/>
     </row>
     <row r="22" spans="1:19">
-      <c r="A22" s="116" t="s">
+      <c r="A22" s="117" t="s">
         <v>225</v>
       </c>
-      <c r="B22" s="116"/>
+      <c r="B22" s="117"/>
       <c r="C22" s="19">
         <f>SUBTOTAL(9,C6:C21)</f>
         <v>162850</v>
@@ -3513,25 +3513,25 @@
       <c r="S22" s="8"/>
     </row>
     <row r="23" spans="1:19">
-      <c r="A23" s="142"/>
-      <c r="B23" s="126"/>
-      <c r="C23" s="126"/>
-      <c r="D23" s="126"/>
-      <c r="E23" s="126"/>
-      <c r="F23" s="126"/>
-      <c r="G23" s="126"/>
-      <c r="H23" s="134"/>
-      <c r="I23" s="129"/>
-      <c r="J23" s="129"/>
-      <c r="K23" s="129"/>
-      <c r="L23" s="129"/>
-      <c r="M23" s="129"/>
-      <c r="N23" s="129"/>
-      <c r="O23" s="129"/>
-      <c r="P23" s="129"/>
-      <c r="Q23" s="129"/>
-      <c r="R23" s="129"/>
-      <c r="S23" s="129"/>
+      <c r="A23" s="143"/>
+      <c r="B23" s="127"/>
+      <c r="C23" s="127"/>
+      <c r="D23" s="127"/>
+      <c r="E23" s="127"/>
+      <c r="F23" s="127"/>
+      <c r="G23" s="127"/>
+      <c r="H23" s="135"/>
+      <c r="I23" s="130"/>
+      <c r="J23" s="130"/>
+      <c r="K23" s="130"/>
+      <c r="L23" s="130"/>
+      <c r="M23" s="130"/>
+      <c r="N23" s="130"/>
+      <c r="O23" s="130"/>
+      <c r="P23" s="130"/>
+      <c r="Q23" s="130"/>
+      <c r="R23" s="130"/>
+      <c r="S23" s="130"/>
     </row>
     <row r="24" spans="1:19">
       <c r="A24" s="24"/>
@@ -3667,10 +3667,10 @@
       <c r="S27" s="8"/>
     </row>
     <row r="28" spans="1:19">
-      <c r="A28" s="116" t="s">
+      <c r="A28" s="117" t="s">
         <v>228</v>
       </c>
-      <c r="B28" s="116"/>
+      <c r="B28" s="117"/>
       <c r="C28" s="19">
         <f>SUBTOTAL(9,C24:C27)</f>
         <v>15000</v>
@@ -3705,25 +3705,25 @@
       <c r="S28" s="8"/>
     </row>
     <row r="29" spans="1:19">
-      <c r="A29" s="142"/>
-      <c r="B29" s="126"/>
-      <c r="C29" s="126"/>
-      <c r="D29" s="126"/>
-      <c r="E29" s="126"/>
-      <c r="F29" s="126"/>
-      <c r="G29" s="126"/>
-      <c r="H29" s="134"/>
-      <c r="I29" s="129"/>
-      <c r="J29" s="129"/>
-      <c r="K29" s="129"/>
-      <c r="L29" s="129"/>
-      <c r="M29" s="129"/>
-      <c r="N29" s="129"/>
-      <c r="O29" s="129"/>
-      <c r="P29" s="129"/>
-      <c r="Q29" s="129"/>
-      <c r="R29" s="129"/>
-      <c r="S29" s="129"/>
+      <c r="A29" s="143"/>
+      <c r="B29" s="127"/>
+      <c r="C29" s="127"/>
+      <c r="D29" s="127"/>
+      <c r="E29" s="127"/>
+      <c r="F29" s="127"/>
+      <c r="G29" s="127"/>
+      <c r="H29" s="135"/>
+      <c r="I29" s="130"/>
+      <c r="J29" s="130"/>
+      <c r="K29" s="130"/>
+      <c r="L29" s="130"/>
+      <c r="M29" s="130"/>
+      <c r="N29" s="130"/>
+      <c r="O29" s="130"/>
+      <c r="P29" s="130"/>
+      <c r="Q29" s="130"/>
+      <c r="R29" s="130"/>
+      <c r="S29" s="130"/>
     </row>
     <row r="30" spans="1:19">
       <c r="A30" s="27" t="s">
@@ -3829,10 +3829,10 @@
       <c r="S32" s="8"/>
     </row>
     <row r="33" spans="1:19">
-      <c r="A33" s="135" t="s">
+      <c r="A33" s="136" t="s">
         <v>232</v>
       </c>
-      <c r="B33" s="135"/>
+      <c r="B33" s="136"/>
       <c r="C33" s="38">
         <f>SUBTOTAL(9,C6:C32)</f>
         <v>216891</v>
@@ -3954,15 +3954,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="15.5">
-      <c r="A1" s="148" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="149"/>
-      <c r="C1" s="149"/>
-      <c r="D1" s="149"/>
-      <c r="E1" s="149"/>
-      <c r="F1" s="149"/>
-      <c r="G1" s="138"/>
+      <c r="A1" s="144" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="145"/>
+      <c r="C1" s="145"/>
+      <c r="D1" s="145"/>
+      <c r="E1" s="145"/>
+      <c r="F1" s="145"/>
+      <c r="G1" s="139"/>
       <c r="H1" s="39"/>
       <c r="I1" s="39"/>
       <c r="J1" s="39"/>
@@ -3977,15 +3977,15 @@
       <c r="S1" s="39"/>
     </row>
     <row r="2" spans="1:19" ht="15.5">
-      <c r="A2" s="150">
+      <c r="A2" s="146">
         <v>2021</v>
       </c>
-      <c r="B2" s="148"/>
-      <c r="C2" s="148"/>
-      <c r="D2" s="148"/>
-      <c r="E2" s="148"/>
-      <c r="F2" s="149"/>
-      <c r="G2" s="138"/>
+      <c r="B2" s="144"/>
+      <c r="C2" s="144"/>
+      <c r="D2" s="144"/>
+      <c r="E2" s="144"/>
+      <c r="F2" s="145"/>
+      <c r="G2" s="139"/>
       <c r="H2" s="39"/>
       <c r="I2" s="39"/>
       <c r="J2" s="39"/>
@@ -4000,15 +4000,15 @@
       <c r="S2" s="39"/>
     </row>
     <row r="3" spans="1:19" ht="15.5">
-      <c r="A3" s="151" t="s">
+      <c r="A3" s="147" t="s">
         <v>238</v>
       </c>
-      <c r="B3" s="151"/>
-      <c r="C3" s="151"/>
-      <c r="D3" s="148"/>
-      <c r="E3" s="148"/>
-      <c r="F3" s="149"/>
-      <c r="G3" s="138"/>
+      <c r="B3" s="147"/>
+      <c r="C3" s="147"/>
+      <c r="D3" s="144"/>
+      <c r="E3" s="144"/>
+      <c r="F3" s="145"/>
+      <c r="G3" s="139"/>
       <c r="H3" s="39"/>
       <c r="I3" s="39"/>
       <c r="J3" s="39"/>
@@ -4082,48 +4082,48 @@
       </c>
     </row>
     <row r="5" spans="1:19" ht="14.5">
-      <c r="A5" s="145"/>
-      <c r="B5" s="146"/>
-      <c r="C5" s="146"/>
-      <c r="D5" s="146"/>
-      <c r="E5" s="146"/>
-      <c r="F5" s="146"/>
-      <c r="G5" s="146"/>
-      <c r="H5" s="143"/>
-      <c r="I5" s="129"/>
-      <c r="J5" s="129"/>
-      <c r="K5" s="129"/>
-      <c r="L5" s="129"/>
-      <c r="M5" s="129"/>
-      <c r="N5" s="129"/>
-      <c r="O5" s="129"/>
-      <c r="P5" s="129"/>
-      <c r="Q5" s="129"/>
-      <c r="R5" s="129"/>
-      <c r="S5" s="129"/>
+      <c r="A5" s="148"/>
+      <c r="B5" s="149"/>
+      <c r="C5" s="149"/>
+      <c r="D5" s="149"/>
+      <c r="E5" s="149"/>
+      <c r="F5" s="149"/>
+      <c r="G5" s="149"/>
+      <c r="H5" s="150"/>
+      <c r="I5" s="130"/>
+      <c r="J5" s="130"/>
+      <c r="K5" s="130"/>
+      <c r="L5" s="130"/>
+      <c r="M5" s="130"/>
+      <c r="N5" s="130"/>
+      <c r="O5" s="130"/>
+      <c r="P5" s="130"/>
+      <c r="Q5" s="130"/>
+      <c r="R5" s="130"/>
+      <c r="S5" s="130"/>
     </row>
     <row r="6" spans="1:19" ht="14.5">
-      <c r="A6" s="145" t="s">
+      <c r="A6" s="148" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="146"/>
-      <c r="C6" s="146"/>
-      <c r="D6" s="146"/>
-      <c r="E6" s="146"/>
-      <c r="F6" s="146"/>
-      <c r="G6" s="146"/>
-      <c r="H6" s="143"/>
-      <c r="I6" s="129"/>
-      <c r="J6" s="129"/>
-      <c r="K6" s="129"/>
-      <c r="L6" s="129"/>
-      <c r="M6" s="129"/>
-      <c r="N6" s="129"/>
-      <c r="O6" s="129"/>
-      <c r="P6" s="129"/>
-      <c r="Q6" s="129"/>
-      <c r="R6" s="129"/>
-      <c r="S6" s="129"/>
+      <c r="B6" s="149"/>
+      <c r="C6" s="149"/>
+      <c r="D6" s="149"/>
+      <c r="E6" s="149"/>
+      <c r="F6" s="149"/>
+      <c r="G6" s="149"/>
+      <c r="H6" s="150"/>
+      <c r="I6" s="130"/>
+      <c r="J6" s="130"/>
+      <c r="K6" s="130"/>
+      <c r="L6" s="130"/>
+      <c r="M6" s="130"/>
+      <c r="N6" s="130"/>
+      <c r="O6" s="130"/>
+      <c r="P6" s="130"/>
+      <c r="Q6" s="130"/>
+      <c r="R6" s="130"/>
+      <c r="S6" s="130"/>
     </row>
     <row r="7" spans="1:19" ht="14.5">
       <c r="A7" s="45" t="s">
@@ -4999,25 +4999,25 @@
       <c r="S32" s="75"/>
     </row>
     <row r="33" spans="1:19" ht="14.5">
-      <c r="A33" s="145"/>
-      <c r="B33" s="126"/>
-      <c r="C33" s="126"/>
-      <c r="D33" s="126"/>
-      <c r="E33" s="126"/>
-      <c r="F33" s="126"/>
-      <c r="G33" s="126"/>
-      <c r="H33" s="147"/>
-      <c r="I33" s="129"/>
-      <c r="J33" s="129"/>
-      <c r="K33" s="129"/>
-      <c r="L33" s="129"/>
-      <c r="M33" s="129"/>
-      <c r="N33" s="129"/>
-      <c r="O33" s="129"/>
-      <c r="P33" s="129"/>
-      <c r="Q33" s="129"/>
-      <c r="R33" s="129"/>
-      <c r="S33" s="129"/>
+      <c r="A33" s="148"/>
+      <c r="B33" s="127"/>
+      <c r="C33" s="127"/>
+      <c r="D33" s="127"/>
+      <c r="E33" s="127"/>
+      <c r="F33" s="127"/>
+      <c r="G33" s="127"/>
+      <c r="H33" s="151"/>
+      <c r="I33" s="130"/>
+      <c r="J33" s="130"/>
+      <c r="K33" s="130"/>
+      <c r="L33" s="130"/>
+      <c r="M33" s="130"/>
+      <c r="N33" s="130"/>
+      <c r="O33" s="130"/>
+      <c r="P33" s="130"/>
+      <c r="Q33" s="130"/>
+      <c r="R33" s="130"/>
+      <c r="S33" s="130"/>
     </row>
     <row r="34" spans="1:19" ht="14.5">
       <c r="A34" s="54" t="s">
@@ -5553,25 +5553,25 @@
       <c r="S48" s="75"/>
     </row>
     <row r="49" spans="1:19" ht="14.5">
-      <c r="A49" s="145"/>
-      <c r="B49" s="129"/>
-      <c r="C49" s="129"/>
-      <c r="D49" s="129"/>
-      <c r="E49" s="129"/>
-      <c r="F49" s="129"/>
-      <c r="G49" s="129"/>
-      <c r="H49" s="143"/>
-      <c r="I49" s="129"/>
-      <c r="J49" s="129"/>
-      <c r="K49" s="129"/>
-      <c r="L49" s="129"/>
-      <c r="M49" s="129"/>
-      <c r="N49" s="129"/>
-      <c r="O49" s="129"/>
-      <c r="P49" s="129"/>
-      <c r="Q49" s="129"/>
-      <c r="R49" s="129"/>
-      <c r="S49" s="129"/>
+      <c r="A49" s="148"/>
+      <c r="B49" s="130"/>
+      <c r="C49" s="130"/>
+      <c r="D49" s="130"/>
+      <c r="E49" s="130"/>
+      <c r="F49" s="130"/>
+      <c r="G49" s="130"/>
+      <c r="H49" s="150"/>
+      <c r="I49" s="130"/>
+      <c r="J49" s="130"/>
+      <c r="K49" s="130"/>
+      <c r="L49" s="130"/>
+      <c r="M49" s="130"/>
+      <c r="N49" s="130"/>
+      <c r="O49" s="130"/>
+      <c r="P49" s="130"/>
+      <c r="Q49" s="130"/>
+      <c r="R49" s="130"/>
+      <c r="S49" s="130"/>
     </row>
     <row r="50" spans="1:19" ht="14.5">
       <c r="A50" s="45" t="s">
@@ -5891,25 +5891,25 @@
       <c r="S58" s="75"/>
     </row>
     <row r="59" spans="1:19" ht="14.5">
-      <c r="A59" s="145"/>
-      <c r="B59" s="129"/>
-      <c r="C59" s="129"/>
-      <c r="D59" s="129"/>
-      <c r="E59" s="129"/>
-      <c r="F59" s="129"/>
-      <c r="G59" s="129"/>
-      <c r="H59" s="143"/>
-      <c r="I59" s="129"/>
-      <c r="J59" s="129"/>
-      <c r="K59" s="129"/>
-      <c r="L59" s="129"/>
-      <c r="M59" s="129"/>
-      <c r="N59" s="129"/>
-      <c r="O59" s="129"/>
-      <c r="P59" s="129"/>
-      <c r="Q59" s="129"/>
-      <c r="R59" s="129"/>
-      <c r="S59" s="129"/>
+      <c r="A59" s="148"/>
+      <c r="B59" s="130"/>
+      <c r="C59" s="130"/>
+      <c r="D59" s="130"/>
+      <c r="E59" s="130"/>
+      <c r="F59" s="130"/>
+      <c r="G59" s="130"/>
+      <c r="H59" s="150"/>
+      <c r="I59" s="130"/>
+      <c r="J59" s="130"/>
+      <c r="K59" s="130"/>
+      <c r="L59" s="130"/>
+      <c r="M59" s="130"/>
+      <c r="N59" s="130"/>
+      <c r="O59" s="130"/>
+      <c r="P59" s="130"/>
+      <c r="Q59" s="130"/>
+      <c r="R59" s="130"/>
+      <c r="S59" s="130"/>
     </row>
     <row r="60" spans="1:19" ht="14.5">
       <c r="A60" s="54" t="s">
@@ -6120,25 +6120,25 @@
       <c r="S65" s="75"/>
     </row>
     <row r="66" spans="1:19" ht="14.5">
-      <c r="A66" s="145"/>
-      <c r="B66" s="129"/>
-      <c r="C66" s="129"/>
-      <c r="D66" s="129"/>
-      <c r="E66" s="129"/>
-      <c r="F66" s="129"/>
-      <c r="G66" s="129"/>
-      <c r="H66" s="143"/>
-      <c r="I66" s="129"/>
-      <c r="J66" s="129"/>
-      <c r="K66" s="129"/>
-      <c r="L66" s="129"/>
-      <c r="M66" s="129"/>
-      <c r="N66" s="129"/>
-      <c r="O66" s="129"/>
-      <c r="P66" s="129"/>
-      <c r="Q66" s="129"/>
-      <c r="R66" s="129"/>
-      <c r="S66" s="129"/>
+      <c r="A66" s="148"/>
+      <c r="B66" s="130"/>
+      <c r="C66" s="130"/>
+      <c r="D66" s="130"/>
+      <c r="E66" s="130"/>
+      <c r="F66" s="130"/>
+      <c r="G66" s="130"/>
+      <c r="H66" s="150"/>
+      <c r="I66" s="130"/>
+      <c r="J66" s="130"/>
+      <c r="K66" s="130"/>
+      <c r="L66" s="130"/>
+      <c r="M66" s="130"/>
+      <c r="N66" s="130"/>
+      <c r="O66" s="130"/>
+      <c r="P66" s="130"/>
+      <c r="Q66" s="130"/>
+      <c r="R66" s="130"/>
+      <c r="S66" s="130"/>
     </row>
     <row r="67" spans="1:19" ht="14.5">
       <c r="A67" s="45" t="s">
@@ -6348,25 +6348,25 @@
       <c r="S72" s="75"/>
     </row>
     <row r="73" spans="1:19" ht="14.5">
-      <c r="A73" s="145"/>
-      <c r="B73" s="129"/>
-      <c r="C73" s="129"/>
-      <c r="D73" s="129"/>
-      <c r="E73" s="129"/>
-      <c r="F73" s="129"/>
-      <c r="G73" s="129"/>
-      <c r="H73" s="143"/>
-      <c r="I73" s="129"/>
-      <c r="J73" s="129"/>
-      <c r="K73" s="129"/>
-      <c r="L73" s="129"/>
-      <c r="M73" s="129"/>
-      <c r="N73" s="129"/>
-      <c r="O73" s="129"/>
-      <c r="P73" s="129"/>
-      <c r="Q73" s="129"/>
-      <c r="R73" s="129"/>
-      <c r="S73" s="129"/>
+      <c r="A73" s="148"/>
+      <c r="B73" s="130"/>
+      <c r="C73" s="130"/>
+      <c r="D73" s="130"/>
+      <c r="E73" s="130"/>
+      <c r="F73" s="130"/>
+      <c r="G73" s="130"/>
+      <c r="H73" s="150"/>
+      <c r="I73" s="130"/>
+      <c r="J73" s="130"/>
+      <c r="K73" s="130"/>
+      <c r="L73" s="130"/>
+      <c r="M73" s="130"/>
+      <c r="N73" s="130"/>
+      <c r="O73" s="130"/>
+      <c r="P73" s="130"/>
+      <c r="Q73" s="130"/>
+      <c r="R73" s="130"/>
+      <c r="S73" s="130"/>
     </row>
     <row r="74" spans="1:19" ht="14.5">
       <c r="A74" s="54" t="s">
@@ -6615,25 +6615,25 @@
       <c r="S80" s="75"/>
     </row>
     <row r="81" spans="1:19" ht="14.5">
-      <c r="A81" s="145"/>
-      <c r="B81" s="126"/>
-      <c r="C81" s="126"/>
-      <c r="D81" s="126"/>
-      <c r="E81" s="126"/>
-      <c r="F81" s="126"/>
-      <c r="G81" s="126"/>
-      <c r="H81" s="147"/>
-      <c r="I81" s="129"/>
-      <c r="J81" s="129"/>
-      <c r="K81" s="129"/>
-      <c r="L81" s="129"/>
-      <c r="M81" s="129"/>
-      <c r="N81" s="129"/>
-      <c r="O81" s="129"/>
-      <c r="P81" s="129"/>
-      <c r="Q81" s="129"/>
-      <c r="R81" s="129"/>
-      <c r="S81" s="129"/>
+      <c r="A81" s="148"/>
+      <c r="B81" s="127"/>
+      <c r="C81" s="127"/>
+      <c r="D81" s="127"/>
+      <c r="E81" s="127"/>
+      <c r="F81" s="127"/>
+      <c r="G81" s="127"/>
+      <c r="H81" s="151"/>
+      <c r="I81" s="130"/>
+      <c r="J81" s="130"/>
+      <c r="K81" s="130"/>
+      <c r="L81" s="130"/>
+      <c r="M81" s="130"/>
+      <c r="N81" s="130"/>
+      <c r="O81" s="130"/>
+      <c r="P81" s="130"/>
+      <c r="Q81" s="130"/>
+      <c r="R81" s="130"/>
+      <c r="S81" s="130"/>
     </row>
     <row r="82" spans="1:19" ht="14.5">
       <c r="A82" s="45" t="s">
@@ -7101,25 +7101,25 @@
       <c r="S94" s="75"/>
     </row>
     <row r="95" spans="1:19" ht="14.5">
-      <c r="A95" s="145"/>
-      <c r="B95" s="126"/>
-      <c r="C95" s="126"/>
-      <c r="D95" s="126"/>
-      <c r="E95" s="126"/>
-      <c r="F95" s="126"/>
-      <c r="G95" s="126"/>
-      <c r="H95" s="143"/>
-      <c r="I95" s="129"/>
-      <c r="J95" s="129"/>
-      <c r="K95" s="129"/>
-      <c r="L95" s="129"/>
-      <c r="M95" s="129"/>
-      <c r="N95" s="129"/>
-      <c r="O95" s="129"/>
-      <c r="P95" s="129"/>
-      <c r="Q95" s="129"/>
-      <c r="R95" s="129"/>
-      <c r="S95" s="129"/>
+      <c r="A95" s="148"/>
+      <c r="B95" s="127"/>
+      <c r="C95" s="127"/>
+      <c r="D95" s="127"/>
+      <c r="E95" s="127"/>
+      <c r="F95" s="127"/>
+      <c r="G95" s="127"/>
+      <c r="H95" s="150"/>
+      <c r="I95" s="130"/>
+      <c r="J95" s="130"/>
+      <c r="K95" s="130"/>
+      <c r="L95" s="130"/>
+      <c r="M95" s="130"/>
+      <c r="N95" s="130"/>
+      <c r="O95" s="130"/>
+      <c r="P95" s="130"/>
+      <c r="Q95" s="130"/>
+      <c r="R95" s="130"/>
+      <c r="S95" s="130"/>
     </row>
     <row r="96" spans="1:19" ht="14.5">
       <c r="A96" s="54" t="s">
@@ -7372,25 +7372,25 @@
       <c r="S102" s="75"/>
     </row>
     <row r="103" spans="1:19" ht="14.5">
-      <c r="A103" s="144"/>
-      <c r="B103" s="126"/>
-      <c r="C103" s="126"/>
-      <c r="D103" s="126"/>
-      <c r="E103" s="126"/>
-      <c r="F103" s="126"/>
-      <c r="G103" s="126"/>
-      <c r="H103" s="143"/>
-      <c r="I103" s="129"/>
-      <c r="J103" s="129"/>
-      <c r="K103" s="129"/>
-      <c r="L103" s="129"/>
-      <c r="M103" s="129"/>
-      <c r="N103" s="129"/>
-      <c r="O103" s="129"/>
-      <c r="P103" s="129"/>
-      <c r="Q103" s="129"/>
-      <c r="R103" s="129"/>
-      <c r="S103" s="129"/>
+      <c r="A103" s="152"/>
+      <c r="B103" s="127"/>
+      <c r="C103" s="127"/>
+      <c r="D103" s="127"/>
+      <c r="E103" s="127"/>
+      <c r="F103" s="127"/>
+      <c r="G103" s="127"/>
+      <c r="H103" s="150"/>
+      <c r="I103" s="130"/>
+      <c r="J103" s="130"/>
+      <c r="K103" s="130"/>
+      <c r="L103" s="130"/>
+      <c r="M103" s="130"/>
+      <c r="N103" s="130"/>
+      <c r="O103" s="130"/>
+      <c r="P103" s="130"/>
+      <c r="Q103" s="130"/>
+      <c r="R103" s="130"/>
+      <c r="S103" s="130"/>
     </row>
     <row r="104" spans="1:19" ht="14.5">
       <c r="A104" s="45" t="s">
@@ -7493,25 +7493,25 @@
       <c r="S106" s="75"/>
     </row>
     <row r="107" spans="1:19" ht="14.5">
-      <c r="A107" s="145"/>
-      <c r="B107" s="126"/>
-      <c r="C107" s="126"/>
-      <c r="D107" s="126"/>
-      <c r="E107" s="126"/>
-      <c r="F107" s="126"/>
-      <c r="G107" s="126"/>
-      <c r="H107" s="143"/>
-      <c r="I107" s="129"/>
-      <c r="J107" s="129"/>
-      <c r="K107" s="129"/>
-      <c r="L107" s="129"/>
-      <c r="M107" s="129"/>
-      <c r="N107" s="129"/>
-      <c r="O107" s="129"/>
-      <c r="P107" s="129"/>
-      <c r="Q107" s="129"/>
-      <c r="R107" s="129"/>
-      <c r="S107" s="129"/>
+      <c r="A107" s="148"/>
+      <c r="B107" s="127"/>
+      <c r="C107" s="127"/>
+      <c r="D107" s="127"/>
+      <c r="E107" s="127"/>
+      <c r="F107" s="127"/>
+      <c r="G107" s="127"/>
+      <c r="H107" s="150"/>
+      <c r="I107" s="130"/>
+      <c r="J107" s="130"/>
+      <c r="K107" s="130"/>
+      <c r="L107" s="130"/>
+      <c r="M107" s="130"/>
+      <c r="N107" s="130"/>
+      <c r="O107" s="130"/>
+      <c r="P107" s="130"/>
+      <c r="Q107" s="130"/>
+      <c r="R107" s="130"/>
+      <c r="S107" s="130"/>
     </row>
     <row r="108" spans="1:19" ht="14.5">
       <c r="A108" s="54" t="s">
@@ -7614,13 +7614,13 @@
       <c r="S110" s="75"/>
     </row>
     <row r="111" spans="1:19" ht="14.5">
-      <c r="A111" s="144"/>
-      <c r="B111" s="126"/>
-      <c r="C111" s="126"/>
-      <c r="D111" s="126"/>
-      <c r="E111" s="126"/>
-      <c r="F111" s="126"/>
-      <c r="G111" s="126"/>
+      <c r="A111" s="152"/>
+      <c r="B111" s="127"/>
+      <c r="C111" s="127"/>
+      <c r="D111" s="127"/>
+      <c r="E111" s="127"/>
+      <c r="F111" s="127"/>
+      <c r="G111" s="127"/>
       <c r="H111" s="75"/>
       <c r="I111" s="75"/>
       <c r="J111" s="75"/>
@@ -7673,36 +7673,36 @@
       <c r="S112" s="75"/>
     </row>
     <row r="113" spans="1:19" ht="14.5">
-      <c r="A113" s="145"/>
-      <c r="B113" s="126"/>
-      <c r="C113" s="126"/>
-      <c r="D113" s="126"/>
-      <c r="E113" s="126"/>
-      <c r="F113" s="126"/>
-      <c r="G113" s="126"/>
-      <c r="H113" s="143"/>
-      <c r="I113" s="129"/>
-      <c r="J113" s="129"/>
-      <c r="K113" s="129"/>
-      <c r="L113" s="129"/>
-      <c r="M113" s="129"/>
-      <c r="N113" s="129"/>
-      <c r="O113" s="129"/>
-      <c r="P113" s="129"/>
-      <c r="Q113" s="129"/>
-      <c r="R113" s="129"/>
-      <c r="S113" s="129"/>
+      <c r="A113" s="148"/>
+      <c r="B113" s="127"/>
+      <c r="C113" s="127"/>
+      <c r="D113" s="127"/>
+      <c r="E113" s="127"/>
+      <c r="F113" s="127"/>
+      <c r="G113" s="127"/>
+      <c r="H113" s="150"/>
+      <c r="I113" s="130"/>
+      <c r="J113" s="130"/>
+      <c r="K113" s="130"/>
+      <c r="L113" s="130"/>
+      <c r="M113" s="130"/>
+      <c r="N113" s="130"/>
+      <c r="O113" s="130"/>
+      <c r="P113" s="130"/>
+      <c r="Q113" s="130"/>
+      <c r="R113" s="130"/>
+      <c r="S113" s="130"/>
     </row>
     <row r="114" spans="1:19" ht="14.5">
-      <c r="A114" s="145" t="s">
+      <c r="A114" s="148" t="s">
         <v>163</v>
       </c>
-      <c r="B114" s="146"/>
-      <c r="C114" s="146"/>
-      <c r="D114" s="146"/>
-      <c r="E114" s="146"/>
-      <c r="F114" s="146"/>
-      <c r="G114" s="146"/>
+      <c r="B114" s="149"/>
+      <c r="C114" s="149"/>
+      <c r="D114" s="149"/>
+      <c r="E114" s="149"/>
+      <c r="F114" s="149"/>
+      <c r="G114" s="149"/>
       <c r="H114" s="75"/>
       <c r="I114" s="75"/>
       <c r="J114" s="75"/>
@@ -7964,25 +7964,25 @@
       <c r="S121" s="75"/>
     </row>
     <row r="122" spans="1:19" ht="14.5">
-      <c r="A122" s="144"/>
-      <c r="B122" s="126"/>
-      <c r="C122" s="126"/>
-      <c r="D122" s="126"/>
-      <c r="E122" s="126"/>
-      <c r="F122" s="126"/>
-      <c r="G122" s="126"/>
-      <c r="H122" s="143"/>
-      <c r="I122" s="129"/>
-      <c r="J122" s="129"/>
-      <c r="K122" s="129"/>
-      <c r="L122" s="129"/>
-      <c r="M122" s="129"/>
-      <c r="N122" s="129"/>
-      <c r="O122" s="129"/>
-      <c r="P122" s="129"/>
-      <c r="Q122" s="129"/>
-      <c r="R122" s="129"/>
-      <c r="S122" s="129"/>
+      <c r="A122" s="152"/>
+      <c r="B122" s="127"/>
+      <c r="C122" s="127"/>
+      <c r="D122" s="127"/>
+      <c r="E122" s="127"/>
+      <c r="F122" s="127"/>
+      <c r="G122" s="127"/>
+      <c r="H122" s="150"/>
+      <c r="I122" s="130"/>
+      <c r="J122" s="130"/>
+      <c r="K122" s="130"/>
+      <c r="L122" s="130"/>
+      <c r="M122" s="130"/>
+      <c r="N122" s="130"/>
+      <c r="O122" s="130"/>
+      <c r="P122" s="130"/>
+      <c r="Q122" s="130"/>
+      <c r="R122" s="130"/>
+      <c r="S122" s="130"/>
     </row>
     <row r="123" spans="1:19" ht="14.5">
       <c r="A123" s="69"/>
@@ -8023,25 +8023,25 @@
       <c r="S123" s="75"/>
     </row>
     <row r="124" spans="1:19" ht="14.5">
-      <c r="A124" s="145"/>
-      <c r="B124" s="126"/>
-      <c r="C124" s="126"/>
-      <c r="D124" s="126"/>
-      <c r="E124" s="126"/>
-      <c r="F124" s="126"/>
-      <c r="G124" s="126"/>
-      <c r="H124" s="143"/>
-      <c r="I124" s="129"/>
-      <c r="J124" s="129"/>
-      <c r="K124" s="129"/>
-      <c r="L124" s="129"/>
-      <c r="M124" s="129"/>
-      <c r="N124" s="129"/>
-      <c r="O124" s="129"/>
-      <c r="P124" s="129"/>
-      <c r="Q124" s="129"/>
-      <c r="R124" s="129"/>
-      <c r="S124" s="129"/>
+      <c r="A124" s="148"/>
+      <c r="B124" s="127"/>
+      <c r="C124" s="127"/>
+      <c r="D124" s="127"/>
+      <c r="E124" s="127"/>
+      <c r="F124" s="127"/>
+      <c r="G124" s="127"/>
+      <c r="H124" s="150"/>
+      <c r="I124" s="130"/>
+      <c r="J124" s="130"/>
+      <c r="K124" s="130"/>
+      <c r="L124" s="130"/>
+      <c r="M124" s="130"/>
+      <c r="N124" s="130"/>
+      <c r="O124" s="130"/>
+      <c r="P124" s="130"/>
+      <c r="Q124" s="130"/>
+      <c r="R124" s="130"/>
+      <c r="S124" s="130"/>
     </row>
     <row r="125" spans="1:19" ht="14.5">
       <c r="A125" s="72"/>
@@ -8234,29 +8234,6 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A5:G5"/>
-    <mergeCell ref="A6:G6"/>
-    <mergeCell ref="H5:S5"/>
-    <mergeCell ref="H6:S6"/>
-    <mergeCell ref="A33:G33"/>
-    <mergeCell ref="H33:S33"/>
-    <mergeCell ref="A49:G49"/>
-    <mergeCell ref="H49:S49"/>
-    <mergeCell ref="H59:S59"/>
-    <mergeCell ref="A66:G66"/>
-    <mergeCell ref="H66:S66"/>
-    <mergeCell ref="A73:G73"/>
-    <mergeCell ref="H73:S73"/>
-    <mergeCell ref="A59:G59"/>
-    <mergeCell ref="H81:S81"/>
-    <mergeCell ref="A95:G95"/>
-    <mergeCell ref="H95:S95"/>
-    <mergeCell ref="A103:G103"/>
-    <mergeCell ref="H103:S103"/>
-    <mergeCell ref="A81:G81"/>
     <mergeCell ref="H107:S107"/>
     <mergeCell ref="A122:G122"/>
     <mergeCell ref="A124:G124"/>
@@ -8267,6 +8244,29 @@
     <mergeCell ref="A107:G107"/>
     <mergeCell ref="A111:G111"/>
     <mergeCell ref="A113:G113"/>
+    <mergeCell ref="H81:S81"/>
+    <mergeCell ref="A95:G95"/>
+    <mergeCell ref="H95:S95"/>
+    <mergeCell ref="A103:G103"/>
+    <mergeCell ref="H103:S103"/>
+    <mergeCell ref="A81:G81"/>
+    <mergeCell ref="H59:S59"/>
+    <mergeCell ref="A66:G66"/>
+    <mergeCell ref="H66:S66"/>
+    <mergeCell ref="A73:G73"/>
+    <mergeCell ref="H73:S73"/>
+    <mergeCell ref="A59:G59"/>
+    <mergeCell ref="H5:S5"/>
+    <mergeCell ref="H6:S6"/>
+    <mergeCell ref="A33:G33"/>
+    <mergeCell ref="H33:S33"/>
+    <mergeCell ref="A49:G49"/>
+    <mergeCell ref="H49:S49"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A5:G5"/>
+    <mergeCell ref="A6:G6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>